<commit_message>
Updated examples with new indexing
</commit_message>
<xml_diff>
--- a/hedcode/data/spreadsheet_data/ExcelMultipleSheets.xlsx
+++ b/hedcode/data/spreadsheet_data/ExcelMultipleSheets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\HEDPython\hed-python\webtools\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HEDExamples\hed-examples\hedcode\data\spreadsheet_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87AD279-418E-4995-873B-7971F6D57BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500"/>
+    <workbookView xWindow="703" yWindow="0" windowWidth="33240" windowHeight="17631" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LKT 8HED3" sheetId="4" r:id="rId1"/>
@@ -255,17 +256,17 @@
     <t>Agent-action, Participant-response, (Halt, Correction)</t>
   </si>
   <si>
-    <t>Subject completes response to perturbation having steered the vehicle back to the center of the lane. Normally this would be tagged with temporal scope, but avoiding definitions here.</t>
-  </si>
-  <si>
     <t>Agent-action, Participant-response, Correction, ((Human-agent, Experiment-participant), (Modify, (Car,Angle)))</t>
+  </si>
+  <si>
+    <t>Subject completes response to perturbation having steered the vehicle back to the center of the lane. Normally this would be tagged with temporal scope but avoiding definitions here.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -350,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -370,28 +371,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -673,14 +668,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.3828125" style="1" customWidth="1"/>
     <col min="2" max="3" width="23.07421875" style="2" customWidth="1"/>
@@ -689,7 +684,7 @@
     <col min="6" max="1026" width="8.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -706,7 +701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.75">
+    <row r="2" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>251</v>
       </c>
@@ -723,7 +718,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.75">
+    <row r="3" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>252</v>
       </c>
@@ -740,7 +735,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="47.05" customHeight="1">
+    <row r="4" spans="1:5" ht="47.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>253</v>
       </c>
@@ -754,10 +749,10 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.75">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>254</v>
       </c>
@@ -768,7 +763,7 @@
         <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>56</v>
@@ -781,14 +776,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.3828125" style="1" customWidth="1"/>
     <col min="2" max="3" width="23.07421875" style="2" customWidth="1"/>
@@ -797,7 +792,7 @@
     <col min="6" max="1026" width="8.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -814,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="58.3">
+    <row r="2" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>251</v>
       </c>
@@ -831,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="58.3">
+    <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>252</v>
       </c>
@@ -848,7 +843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="47.05" customHeight="1">
+    <row r="4" spans="1:5" ht="47.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>253</v>
       </c>
@@ -865,7 +860,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58.3">
+    <row r="5" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>254</v>
       </c>
@@ -889,14 +884,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="26.3828125" customWidth="1"/>
     <col min="2" max="2" width="25.61328125" customWidth="1"/>
@@ -905,7 +900,7 @@
     <col min="5" max="1025" width="8.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -915,71 +910,71 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="87.45">
-      <c r="A2" s="8">
+    <row r="2" spans="1:4" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="44.6">
-      <c r="A3" s="8">
+    <row r="3" spans="1:4" ht="44.6" x14ac:dyDescent="0.4">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.75">
-      <c r="A4" s="8">
+    <row r="4" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A4" s="7">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="58.3">
-      <c r="A5" s="8">
+    <row r="5" spans="1:4" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A5" s="7">
         <v>32</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="8">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="7">
         <v>64</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
@@ -996,121 +991,121 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.61328125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="24.84375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="69.53515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="118.07421875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="17.61328125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.84375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="69.53515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="118.07421875" style="11" customWidth="1"/>
     <col min="5" max="5" width="55.07421875" customWidth="1"/>
     <col min="6" max="1025" width="8.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.15">
-      <c r="A2" s="8">
+    <row r="2" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="102">
-      <c r="A3" s="8">
+    <row r="3" spans="1:5" ht="102" x14ac:dyDescent="0.4">
+      <c r="A3" s="7">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="102">
-      <c r="A4" s="8">
+    <row r="4" spans="1:5" ht="102" x14ac:dyDescent="0.4">
+      <c r="A4" s="7">
         <v>12</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="87.45">
-      <c r="A5" s="8">
+    <row r="5" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A5" s="7">
         <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="87.45">
-      <c r="A6" s="8">
+    <row r="6" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A6" s="7">
         <v>14</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="8">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="7">
         <v>55</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>